<commit_message>
save procedure done start 진행중
</commit_message>
<xml_diff>
--- a/atr.xlsx
+++ b/atr.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,6 +433,45 @@
           <t>Hz</t>
         </is>
       </c>
+      <c r="C1" t="n">
+        <v>6000000000</v>
+      </c>
+      <c r="D1" t="n">
+        <v>7000000000</v>
+      </c>
+      <c r="E1" t="n">
+        <v>8000000000</v>
+      </c>
+      <c r="F1" t="n">
+        <v>9000000000</v>
+      </c>
+      <c r="G1" t="n">
+        <v>10000000000</v>
+      </c>
+      <c r="H1" t="n">
+        <v>11000000000</v>
+      </c>
+      <c r="I1" t="n">
+        <v>12000000000</v>
+      </c>
+      <c r="J1" t="n">
+        <v>13000000000</v>
+      </c>
+      <c r="K1" t="n">
+        <v>14000000000</v>
+      </c>
+      <c r="L1" t="n">
+        <v>15000000000</v>
+      </c>
+      <c r="M1" t="n">
+        <v>16000000000</v>
+      </c>
+      <c r="N1" t="n">
+        <v>17000000000</v>
+      </c>
+      <c r="O1" t="n">
+        <v>18000000000</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -445,6 +484,45 @@
           <t>dBm</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>8</v>
+      </c>
+      <c r="L2" t="n">
+        <v>9</v>
+      </c>
+      <c r="M2" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" t="n">
+        <v>11</v>
+      </c>
+      <c r="O2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -457,6 +535,45 @@
           <t>W</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.001258925411794167</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.001584893192461114</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.001995262314968879</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.00251188643150958</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.003162277660168379</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.003981071705534973</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.005011872336272722</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.006309573444801934</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.007943282347242816</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.01258925411794167</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.01584893192461113</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -468,6 +585,45 @@
         <is>
           <t>A</t>
         </is>
+      </c>
+      <c r="C4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" t="n">
+        <v>7</v>
+      </c>
+      <c r="J4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
동작 70%정도 완료 input, output offset 구현완료
</commit_message>
<xml_diff>
--- a/atr.xlsx
+++ b/atr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ATR" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OFFSET" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,325 +440,110 @@
         <v>1100000000</v>
       </c>
       <c r="D1" t="n">
+        <v>1150000000</v>
+      </c>
+      <c r="E1" t="n">
         <v>1200000000</v>
       </c>
-      <c r="E1" t="n">
+      <c r="F1" t="n">
+        <v>1250000000</v>
+      </c>
+      <c r="G1" t="n">
         <v>1300000000</v>
       </c>
-      <c r="F1" t="n">
+      <c r="H1" t="n">
         <v>1400000000</v>
       </c>
-      <c r="G1" t="n">
+      <c r="I1" t="n">
         <v>1500000000</v>
       </c>
-      <c r="H1" t="n">
+      <c r="J1" t="n">
         <v>1600000000</v>
       </c>
-      <c r="I1" t="n">
-        <v>1700000000</v>
-      </c>
-      <c r="J1" t="n">
+      <c r="K1" t="n">
         <v>1800000000</v>
       </c>
-      <c r="K1" t="n">
-        <v>1900000000</v>
-      </c>
       <c r="L1" t="n">
-        <v>2000000000</v>
-      </c>
-      <c r="M1" t="n">
-        <v>2100000000</v>
-      </c>
-      <c r="N1" t="n">
-        <v>2200000000</v>
-      </c>
-      <c r="O1" t="n">
-        <v>2300000000</v>
+        <v>1990000000</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>p1</t>
+          <t>input offset</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dBm</t>
+          <t>dB</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0</v>
+        <v>-10.6</v>
       </c>
       <c r="D2" t="n">
-        <v>-0</v>
+        <v>-10.7</v>
       </c>
       <c r="E2" t="n">
-        <v>-0</v>
+        <v>-10.7</v>
       </c>
       <c r="F2" t="n">
-        <v>-0</v>
+        <v>-10.7</v>
       </c>
       <c r="G2" t="n">
-        <v>-0</v>
+        <v>-10.7</v>
       </c>
       <c r="H2" t="n">
-        <v>-0</v>
+        <v>-10.7</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>-10.8</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-10.8</v>
       </c>
       <c r="K2" t="n">
-        <v>-0</v>
+        <v>-10.9</v>
       </c>
       <c r="L2" t="n">
-        <v>-0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-0</v>
+        <v>-10.9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>input dBm</t>
+          <t>output offset</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dBm</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>input watt</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>input current</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>p_sat dBm</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>dBm</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>50.19</v>
-      </c>
-      <c r="D6" t="n">
-        <v>49.94</v>
-      </c>
-      <c r="E6" t="n">
-        <v>49.99</v>
-      </c>
-      <c r="F6" t="n">
-        <v>50.06</v>
-      </c>
-      <c r="G6" t="n">
-        <v>50.11</v>
-      </c>
-      <c r="H6" t="n">
-        <v>50.13</v>
-      </c>
-      <c r="I6" t="n">
-        <v>50.33</v>
-      </c>
-      <c r="J6" t="n">
-        <v>50.37</v>
-      </c>
-      <c r="K6" t="n">
-        <v>50.59</v>
-      </c>
-      <c r="L6" t="n">
-        <v>50.71</v>
-      </c>
-      <c r="M6" t="n">
-        <v>50.83</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>p_sat watt</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>104.47202192208</v>
-      </c>
-      <c r="D7" t="n">
-        <v>98.627948563121</v>
-      </c>
-      <c r="E7" t="n">
-        <v>99.77000638225546</v>
-      </c>
-      <c r="F7" t="n">
-        <v>101.391138573668</v>
-      </c>
-      <c r="G7" t="n">
-        <v>102.5651926251408</v>
-      </c>
-      <c r="H7" t="n">
-        <v>103.0386120441616</v>
-      </c>
-      <c r="I7" t="n">
-        <v>107.8946722229827</v>
-      </c>
-      <c r="J7" t="n">
-        <v>108.8930093333433</v>
-      </c>
-      <c r="K7" t="n">
-        <v>114.5512941445536</v>
-      </c>
-      <c r="L7" t="n">
-        <v>117.7605973520807</v>
-      </c>
-      <c r="M7" t="n">
-        <v>121.0598133550483</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>p_sat current</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>overdrive dBm</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>dBm</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>49.93</v>
-      </c>
-      <c r="D9" t="n">
-        <v>49.98</v>
-      </c>
-      <c r="E9" t="n">
-        <v>50.03</v>
-      </c>
-      <c r="F9" t="n">
-        <v>50.08</v>
-      </c>
-      <c r="G9" t="n">
-        <v>50.09</v>
-      </c>
-      <c r="H9" t="n">
-        <v>50.15</v>
-      </c>
-      <c r="I9" t="n">
-        <v>50.34</v>
-      </c>
-      <c r="J9" t="n">
-        <v>50.43</v>
-      </c>
-      <c r="K9" t="n">
-        <v>50.63</v>
-      </c>
-      <c r="L9" t="n">
-        <v>50.78</v>
-      </c>
-      <c r="M9" t="n">
-        <v>50.83</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>overdrive watt</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>98.40111057611345</v>
-      </c>
-      <c r="D10" t="n">
-        <v>99.54054173515254</v>
-      </c>
-      <c r="E10" t="n">
-        <v>100.6931668851804</v>
-      </c>
-      <c r="F10" t="n">
-        <v>101.8591388054117</v>
-      </c>
-      <c r="G10" t="n">
-        <v>102.0939483707681</v>
-      </c>
-      <c r="H10" t="n">
-        <v>103.5142166679343</v>
-      </c>
-      <c r="I10" t="n">
-        <v>108.143395129794</v>
-      </c>
-      <c r="J10" t="n">
-        <v>110.4078619902074</v>
-      </c>
-      <c r="K10" t="n">
-        <v>115.6112242192101</v>
-      </c>
-      <c r="L10" t="n">
-        <v>119.6740531307244</v>
-      </c>
-      <c r="M10" t="n">
-        <v>121.0598133550483</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>overdrive current</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="C3" t="n">
+        <v>-10.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-10.7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-10.7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-10.7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-10.7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-10.7</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-10.8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-10.8</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-10.9</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-10.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>